<commit_message>
latest update to pipeline
</commit_message>
<xml_diff>
--- a/data/total_demand_analysis_results_from_R_table.xlsx
+++ b/data/total_demand_analysis_results_from_R_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\methode_de_prevision_60638\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90868B9F-5CE7-4C6B-86C3-004204C0E623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED6AEED-761C-4993-9CEF-D23F6E072E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BDD8B59D-2511-412D-A817-87AA02FD937E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
     <t>NORTH</t>
   </si>
@@ -902,11 +902,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
-              <a:t>Delta</a:t>
+              <a:t>Evolution annuelle en %</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-CA" baseline="0"/>
-              <a:t> Mean Daily Demand Over Time (%)</a:t>
+              <a:t> de la demande lissee par annee/region</a:t>
             </a:r>
             <a:endParaRPr lang="en-CA"/>
           </a:p>
@@ -1628,11 +1628,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
-              <a:t>Average</a:t>
+              <a:t>Moyenne</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-CA" baseline="0"/>
-              <a:t> Daily Electric Demand (MW) Per Season</a:t>
+              <a:t> de demande journaliere d'electricite en MWh par saison</a:t>
             </a:r>
             <a:endParaRPr lang="en-CA"/>
           </a:p>
@@ -2214,11 +2214,411 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
-              <a:t>Daily</a:t>
+              <a:t>Evolution en pourcentage de la demande journaliere d'electricite sur periode 2012 - 2021</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Total!$R$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2012 to 2021</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.5462668816039986E-17"/>
+                  <c:y val="-5.0925561388159811E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-DC36-4719-8D57-818E81C18A5F}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Total!$Q$7:$Q$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>DELTA NORTH (%)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DELTA EAST (%)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DELTA NCENT (%)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DELTA SOMME (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Total!$R$7:$R$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-0.81627107727452164</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.996174814616236</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8159841091093245</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7762880728319663</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DC36-4719-8D57-818E81C18A5F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1032491919"/>
+        <c:axId val="1032489007"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1032491919"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1032489007"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1032489007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1032491919"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Analyse</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-CA" baseline="0"/>
-              <a:t> Electric Demand Standard Deviation Per Season</a:t>
+              <a:t> de la variabilite par l'ecart type par saison sur periode 2012 2021 en MWh</a:t>
             </a:r>
             <a:endParaRPr lang="en-CA"/>
           </a:p>
@@ -2917,6 +3317,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4466,6 +4906,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5086,6 +6029,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>375708</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>94192</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>164042</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>138642</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5647A1F7-210B-492E-8205-80831FD3616C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5432,10 +6411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC977E8A-71B6-4A0F-BB3F-FA278B8686D0}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5450,9 +6429,10 @@
     <col min="9" max="9" width="13.90625" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="18" max="18" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="3">
         <v>2012</v>
@@ -5485,7 +6465,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -5520,7 +6500,7 @@
         <v>19711.080000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -5555,7 +6535,7 @@
         <v>39502.519999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -5590,7 +6570,7 @@
         <v>322218</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -5625,7 +6605,7 @@
         <v>381431.6</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="3">
         <v>2012</v>
@@ -5660,8 +6640,12 @@
       <c r="L6" t="s">
         <v>8</v>
       </c>
+      <c r="P6" s="2"/>
+      <c r="R6" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5674,7 +6658,7 @@
         <v>1.6846723996517903</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:K7" si="0">100* ((D2-C2)/C2)</f>
+        <f t="shared" ref="D7:J7" si="0">100* ((D2-C2)/C2)</f>
         <v>-1.7468242932283766E-2</v>
       </c>
       <c r="E7">
@@ -5709,8 +6693,14 @@
         <f>100*((K2-B2)/B2)</f>
         <v>-0.81627107727452164</v>
       </c>
+      <c r="Q7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R7">
+        <v>-0.81627107727452164</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -5758,8 +6748,14 @@
         <f t="shared" ref="L8:L10" si="2">100*((K3-B3)/B3)</f>
         <v>21.996174814616236</v>
       </c>
+      <c r="Q8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R8">
+        <v>21.996174814616236</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5807,8 +6803,14 @@
         <f t="shared" si="2"/>
         <v>6.8159841091093245</v>
       </c>
+      <c r="Q9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9">
+        <v>6.8159841091093245</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -5854,6 +6856,12 @@
       </c>
       <c r="L10" s="4">
         <f t="shared" si="2"/>
+        <v>7.7762880728319663</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R10">
         <v>7.7762880728319663</v>
       </c>
     </row>
@@ -5953,7 +6961,7 @@
   <dimension ref="B1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>